<commit_message>
Branch 2 initial commit
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sri/Library/Mobile Documents/com~apple~CloudDocs/dev/xlAutomationTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1495C8E6-E71F-DF47-8E4D-24F86BEF574F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CA0112-EF41-7343-8960-A28FFE1181D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32700" yWindow="1060" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8129,6 +8129,865 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Revenue!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Revenue!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-90CA-F742-9B97-2A9794B7C70E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="259961392"/>
+        <c:axId val="260270512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="259961392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="260270512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="260270512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="259961392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ECDAE78-DF17-56CD-4A24-5492D253F2F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8418,8 +9277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E907"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B31"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8769,6 +9628,9 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32">
+        <v>1000</v>
+      </c>
       <c r="C32" t="s">
         <v>32</v>
       </c>
@@ -8777,6 +9639,9 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33">
+        <v>2000</v>
+      </c>
       <c r="C33" t="s">
         <v>33</v>
       </c>
@@ -8785,6 +9650,9 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34">
+        <v>3000</v>
+      </c>
       <c r="C34" t="s">
         <v>34</v>
       </c>
@@ -8793,6 +9661,9 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35">
+        <v>4000</v>
+      </c>
       <c r="C35" t="s">
         <v>35</v>
       </c>
@@ -8801,6 +9672,9 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36">
+        <v>5000</v>
+      </c>
       <c r="C36" t="s">
         <v>36</v>
       </c>
@@ -8809,6 +9683,9 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37">
+        <v>6000</v>
+      </c>
       <c r="C37" t="s">
         <v>37</v>
       </c>
@@ -8817,6 +9694,9 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38">
+        <v>7000</v>
+      </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
@@ -8825,6 +9705,9 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39">
+        <v>8000</v>
+      </c>
       <c r="C39" t="s">
         <v>39</v>
       </c>
@@ -8833,6 +9716,9 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40">
+        <v>9000</v>
+      </c>
       <c r="C40" t="s">
         <v>40</v>
       </c>
@@ -8841,6 +9727,9 @@
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="B41">
+        <v>10000</v>
+      </c>
       <c r="C41" t="s">
         <v>41</v>
       </c>
@@ -8849,6 +9738,9 @@
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="B42">
+        <v>11000</v>
+      </c>
       <c r="C42" t="s">
         <v>42</v>
       </c>
@@ -8857,6 +9749,9 @@
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43">
+        <v>12000</v>
+      </c>
       <c r="C43" t="s">
         <v>43</v>
       </c>
@@ -8865,6 +9760,9 @@
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44">
+        <v>13000</v>
+      </c>
       <c r="C44" t="s">
         <v>44</v>
       </c>
@@ -8873,6 +9771,9 @@
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45">
+        <v>14000</v>
+      </c>
       <c r="C45" t="s">
         <v>45</v>
       </c>
@@ -8881,6 +9782,9 @@
       <c r="A46">
         <v>45</v>
       </c>
+      <c r="B46">
+        <v>15000</v>
+      </c>
       <c r="C46" t="s">
         <v>46</v>
       </c>
@@ -8889,6 +9793,9 @@
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47">
+        <v>16000</v>
+      </c>
       <c r="C47" t="s">
         <v>47</v>
       </c>
@@ -8897,6 +9804,9 @@
       <c r="A48">
         <v>47</v>
       </c>
+      <c r="B48">
+        <v>17000</v>
+      </c>
       <c r="C48" t="s">
         <v>48</v>
       </c>
@@ -8905,6 +9815,9 @@
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49">
+        <v>18000</v>
+      </c>
       <c r="C49" t="s">
         <v>49</v>
       </c>
@@ -8913,6 +9826,9 @@
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50">
+        <v>19000</v>
+      </c>
       <c r="C50" t="s">
         <v>50</v>
       </c>
@@ -8921,6 +9837,9 @@
       <c r="A51">
         <v>50</v>
       </c>
+      <c r="B51">
+        <v>20000</v>
+      </c>
       <c r="C51" t="s">
         <v>51</v>
       </c>
@@ -8929,6 +9848,9 @@
       <c r="A52">
         <v>51</v>
       </c>
+      <c r="B52">
+        <v>21000</v>
+      </c>
       <c r="C52" t="s">
         <v>52</v>
       </c>
@@ -8937,6 +9859,9 @@
       <c r="A53">
         <v>52</v>
       </c>
+      <c r="B53">
+        <v>22000</v>
+      </c>
       <c r="C53" t="s">
         <v>53</v>
       </c>
@@ -8945,6 +9870,9 @@
       <c r="A54">
         <v>53</v>
       </c>
+      <c r="B54">
+        <v>23000</v>
+      </c>
       <c r="C54" t="s">
         <v>54</v>
       </c>
@@ -8953,6 +9881,9 @@
       <c r="A55">
         <v>54</v>
       </c>
+      <c r="B55">
+        <v>24000</v>
+      </c>
       <c r="C55" t="s">
         <v>55</v>
       </c>
@@ -8961,6 +9892,9 @@
       <c r="A56">
         <v>55</v>
       </c>
+      <c r="B56">
+        <v>25000</v>
+      </c>
       <c r="C56" t="s">
         <v>56</v>
       </c>
@@ -8969,6 +9903,9 @@
       <c r="A57">
         <v>56</v>
       </c>
+      <c r="B57">
+        <v>26000</v>
+      </c>
       <c r="C57" t="s">
         <v>57</v>
       </c>
@@ -8977,6 +9914,9 @@
       <c r="A58">
         <v>57</v>
       </c>
+      <c r="B58">
+        <v>27000</v>
+      </c>
       <c r="C58" t="s">
         <v>58</v>
       </c>
@@ -8985,6 +9925,9 @@
       <c r="A59">
         <v>58</v>
       </c>
+      <c r="B59">
+        <v>28000</v>
+      </c>
       <c r="C59" t="s">
         <v>59</v>
       </c>
@@ -8993,6 +9936,9 @@
       <c r="A60">
         <v>59</v>
       </c>
+      <c r="B60">
+        <v>29000</v>
+      </c>
       <c r="C60" t="s">
         <v>60</v>
       </c>
@@ -9001,6 +9947,9 @@
       <c r="A61">
         <v>60</v>
       </c>
+      <c r="B61">
+        <v>30000</v>
+      </c>
       <c r="C61" t="s">
         <v>61</v>
       </c>
@@ -9009,6 +9958,9 @@
       <c r="A62">
         <v>61</v>
       </c>
+      <c r="B62">
+        <v>1000</v>
+      </c>
       <c r="C62" t="s">
         <v>62</v>
       </c>
@@ -9017,6 +9969,9 @@
       <c r="A63">
         <v>62</v>
       </c>
+      <c r="B63">
+        <v>2000</v>
+      </c>
       <c r="C63" t="s">
         <v>63</v>
       </c>
@@ -9025,6 +9980,9 @@
       <c r="A64">
         <v>63</v>
       </c>
+      <c r="B64">
+        <v>3000</v>
+      </c>
       <c r="C64" t="s">
         <v>64</v>
       </c>
@@ -9033,6 +9991,9 @@
       <c r="A65">
         <v>64</v>
       </c>
+      <c r="B65">
+        <v>4000</v>
+      </c>
       <c r="C65" t="s">
         <v>65</v>
       </c>
@@ -9041,6 +10002,9 @@
       <c r="A66">
         <v>65</v>
       </c>
+      <c r="B66">
+        <v>5000</v>
+      </c>
       <c r="C66" t="s">
         <v>66</v>
       </c>
@@ -9049,6 +10013,9 @@
       <c r="A67">
         <v>66</v>
       </c>
+      <c r="B67">
+        <v>6000</v>
+      </c>
       <c r="C67" t="s">
         <v>67</v>
       </c>
@@ -9057,6 +10024,9 @@
       <c r="A68">
         <v>67</v>
       </c>
+      <c r="B68">
+        <v>7000</v>
+      </c>
       <c r="C68" t="s">
         <v>68</v>
       </c>
@@ -9065,6 +10035,9 @@
       <c r="A69">
         <v>68</v>
       </c>
+      <c r="B69">
+        <v>8000</v>
+      </c>
       <c r="C69" t="s">
         <v>69</v>
       </c>
@@ -9073,6 +10046,9 @@
       <c r="A70">
         <v>69</v>
       </c>
+      <c r="B70">
+        <v>9000</v>
+      </c>
       <c r="C70" t="s">
         <v>70</v>
       </c>
@@ -9081,6 +10057,9 @@
       <c r="A71">
         <v>70</v>
       </c>
+      <c r="B71">
+        <v>10000</v>
+      </c>
       <c r="C71" t="s">
         <v>71</v>
       </c>
@@ -9089,6 +10068,9 @@
       <c r="A72">
         <v>71</v>
       </c>
+      <c r="B72">
+        <v>11000</v>
+      </c>
       <c r="C72" t="s">
         <v>72</v>
       </c>
@@ -9097,6 +10079,9 @@
       <c r="A73">
         <v>72</v>
       </c>
+      <c r="B73">
+        <v>12000</v>
+      </c>
       <c r="C73" t="s">
         <v>73</v>
       </c>
@@ -9105,6 +10090,9 @@
       <c r="A74">
         <v>73</v>
       </c>
+      <c r="B74">
+        <v>13000</v>
+      </c>
       <c r="C74" t="s">
         <v>74</v>
       </c>
@@ -9113,6 +10101,9 @@
       <c r="A75">
         <v>74</v>
       </c>
+      <c r="B75">
+        <v>14000</v>
+      </c>
       <c r="C75" t="s">
         <v>75</v>
       </c>
@@ -9121,6 +10112,9 @@
       <c r="A76">
         <v>75</v>
       </c>
+      <c r="B76">
+        <v>15000</v>
+      </c>
       <c r="C76" t="s">
         <v>76</v>
       </c>
@@ -9129,6 +10123,9 @@
       <c r="A77">
         <v>76</v>
       </c>
+      <c r="B77">
+        <v>16000</v>
+      </c>
       <c r="C77" t="s">
         <v>77</v>
       </c>
@@ -9137,6 +10134,9 @@
       <c r="A78">
         <v>77</v>
       </c>
+      <c r="B78">
+        <v>17000</v>
+      </c>
       <c r="C78" t="s">
         <v>78</v>
       </c>
@@ -9145,6 +10145,9 @@
       <c r="A79">
         <v>78</v>
       </c>
+      <c r="B79">
+        <v>18000</v>
+      </c>
       <c r="C79" t="s">
         <v>79</v>
       </c>
@@ -9153,6 +10156,9 @@
       <c r="A80">
         <v>79</v>
       </c>
+      <c r="B80">
+        <v>19000</v>
+      </c>
       <c r="C80" t="s">
         <v>80</v>
       </c>
@@ -9161,6 +10167,9 @@
       <c r="A81">
         <v>80</v>
       </c>
+      <c r="B81">
+        <v>20000</v>
+      </c>
       <c r="C81" t="s">
         <v>81</v>
       </c>
@@ -9169,6 +10178,9 @@
       <c r="A82">
         <v>81</v>
       </c>
+      <c r="B82">
+        <v>21000</v>
+      </c>
       <c r="C82" t="s">
         <v>82</v>
       </c>
@@ -9177,6 +10189,9 @@
       <c r="A83">
         <v>82</v>
       </c>
+      <c r="B83">
+        <v>22000</v>
+      </c>
       <c r="C83" t="s">
         <v>83</v>
       </c>
@@ -9185,6 +10200,9 @@
       <c r="A84">
         <v>83</v>
       </c>
+      <c r="B84">
+        <v>23000</v>
+      </c>
       <c r="C84" t="s">
         <v>84</v>
       </c>
@@ -9193,6 +10211,9 @@
       <c r="A85">
         <v>84</v>
       </c>
+      <c r="B85">
+        <v>24000</v>
+      </c>
       <c r="C85" t="s">
         <v>85</v>
       </c>
@@ -9201,6 +10222,9 @@
       <c r="A86">
         <v>85</v>
       </c>
+      <c r="B86">
+        <v>25000</v>
+      </c>
       <c r="C86" t="s">
         <v>86</v>
       </c>
@@ -9209,6 +10233,9 @@
       <c r="A87">
         <v>86</v>
       </c>
+      <c r="B87">
+        <v>26000</v>
+      </c>
       <c r="C87" t="s">
         <v>87</v>
       </c>
@@ -9217,6 +10244,9 @@
       <c r="A88">
         <v>87</v>
       </c>
+      <c r="B88">
+        <v>27000</v>
+      </c>
       <c r="C88" t="s">
         <v>88</v>
       </c>
@@ -9225,6 +10255,9 @@
       <c r="A89">
         <v>88</v>
       </c>
+      <c r="B89">
+        <v>28000</v>
+      </c>
       <c r="C89" t="s">
         <v>89</v>
       </c>
@@ -9233,6 +10266,9 @@
       <c r="A90">
         <v>89</v>
       </c>
+      <c r="B90">
+        <v>29000</v>
+      </c>
       <c r="C90" t="s">
         <v>90</v>
       </c>
@@ -9241,6 +10277,9 @@
       <c r="A91">
         <v>90</v>
       </c>
+      <c r="B91">
+        <v>30000</v>
+      </c>
       <c r="C91" t="s">
         <v>91</v>
       </c>
@@ -9249,6 +10288,9 @@
       <c r="A92">
         <v>91</v>
       </c>
+      <c r="B92">
+        <v>31000</v>
+      </c>
       <c r="C92" t="s">
         <v>92</v>
       </c>
@@ -9257,6 +10299,9 @@
       <c r="A93">
         <v>92</v>
       </c>
+      <c r="B93">
+        <v>32000</v>
+      </c>
       <c r="C93" t="s">
         <v>93</v>
       </c>
@@ -9265,6 +10310,9 @@
       <c r="A94">
         <v>93</v>
       </c>
+      <c r="B94">
+        <v>33000</v>
+      </c>
       <c r="C94" t="s">
         <v>94</v>
       </c>
@@ -9273,6 +10321,9 @@
       <c r="A95">
         <v>94</v>
       </c>
+      <c r="B95">
+        <v>34000</v>
+      </c>
       <c r="C95" t="s">
         <v>95</v>
       </c>
@@ -9281,6 +10332,9 @@
       <c r="A96">
         <v>95</v>
       </c>
+      <c r="B96">
+        <v>35000</v>
+      </c>
       <c r="C96" t="s">
         <v>96</v>
       </c>
@@ -9289,6 +10343,9 @@
       <c r="A97">
         <v>96</v>
       </c>
+      <c r="B97">
+        <v>36000</v>
+      </c>
       <c r="C97" t="s">
         <v>97</v>
       </c>
@@ -9297,6 +10354,9 @@
       <c r="A98">
         <v>97</v>
       </c>
+      <c r="B98">
+        <v>37000</v>
+      </c>
       <c r="C98" t="s">
         <v>98</v>
       </c>
@@ -9305,6 +10365,9 @@
       <c r="A99">
         <v>98</v>
       </c>
+      <c r="B99">
+        <v>38000</v>
+      </c>
       <c r="C99" t="s">
         <v>99</v>
       </c>
@@ -9313,6 +10376,9 @@
       <c r="A100">
         <v>99</v>
       </c>
+      <c r="B100">
+        <v>39000</v>
+      </c>
       <c r="C100" t="s">
         <v>100</v>
       </c>
@@ -9320,6 +10386,9 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
+      </c>
+      <c r="B101">
+        <v>40000</v>
       </c>
       <c r="C101" t="s">
         <v>101</v>
@@ -19683,7 +20752,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E1" sqref="E1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19805,6 +20874,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>